<commit_message>
Conexão feita e Update em Andamento
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06182EA-3AED-4007-8239-1B1116B21108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FA8E3D-EF70-4BC2-A6CE-F42C4298AFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>CheckPoint de Python</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Felipe</t>
+  </si>
+  <si>
+    <t>Andamento (50%)</t>
   </si>
 </sst>
 </file>
@@ -147,17 +150,17 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -443,203 +446,193 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G9" sqref="G9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="C14:D14"/>
@@ -650,9 +643,19 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update e Delete quase prontos
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Documents\FIAP\Python\Provas\CP6-Py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADE1F8C-1CB5-4E33-B8BF-1DC6A0C0346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3C4A80-6441-42AB-AC3B-D4E516A51545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>CheckPoint de Python</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Andamento (90%)</t>
+  </si>
+  <si>
+    <t>Chaves</t>
+  </si>
+  <si>
+    <t>Andamento (50%)</t>
   </si>
 </sst>
 </file>
@@ -148,19 +154,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -446,23 +451,23 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:I6"/>
+      <selection activeCell="D9" sqref="D9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -482,158 +487,139 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D2:F2"/>
@@ -647,19 +633,6 @@
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>